<commit_message>
correct pdf and add jade
</commit_message>
<xml_diff>
--- a/FinalProject/material.xlsx
+++ b/FinalProject/material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codes\games101\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD899CC8-9EDA-48F3-A3CA-494D033D7362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F558D65-2149-4013-8E8D-FBD20B109D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5715" yWindow="4635" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>Apple</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,6 +84,10 @@
   </si>
   <si>
     <t>Skin2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jade</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4:W5"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -593,27 +597,27 @@
         <v>0.97648261758691202</v>
       </c>
       <c r="R3">
-        <f>L3 * SQRT(3 * (1 - O3))</f>
+        <f t="shared" ref="R3:T6" si="0">L3 * SQRT(3 * (1 - O3))</f>
         <v>0.14365583872575802</v>
       </c>
       <c r="S3">
-        <f>M3 * SQRT(3 * (1 - P3))</f>
+        <f t="shared" si="0"/>
         <v>0.15624557593737121</v>
       </c>
       <c r="T3">
-        <f>N3 * SQRT(3 * (1 - Q3))</f>
+        <f t="shared" si="0"/>
         <v>0.51954595561894279</v>
       </c>
       <c r="U3">
-        <f xml:space="preserve"> 1 / R3</f>
+        <f t="shared" ref="U3:W6" si="1" xml:space="preserve"> 1 / R3</f>
         <v>6.9610814908054017</v>
       </c>
       <c r="V3">
-        <f xml:space="preserve"> 1 / S3</f>
+        <f t="shared" si="1"/>
         <v>6.4001812147361896</v>
       </c>
       <c r="W3">
-        <f xml:space="preserve"> 1 / T3</f>
+        <f t="shared" si="1"/>
         <v>1.9247575487498216</v>
       </c>
     </row>
@@ -660,15 +664,15 @@
         <v>2.6241000000000003</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N5" si="0" xml:space="preserve"> D4 + G4</f>
+        <f t="shared" ref="N4:N6" si="2" xml:space="preserve"> D4 + G4</f>
         <v>3.0070999999999999</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O5" si="1">B4 / L4</f>
+        <f t="shared" ref="O4:O6" si="3">B4 / L4</f>
         <v>0.99904201450663743</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P5" si="2">C4 / M4</f>
+        <f t="shared" ref="P4:P6" si="4">C4 / M4</f>
         <v>0.99843755954422464</v>
       </c>
       <c r="Q4">
@@ -676,27 +680,27 @@
         <v>0.99763892121977993</v>
       </c>
       <c r="R4">
-        <f>L4 * SQRT(3 * (1 - O4))</f>
+        <f t="shared" si="0"/>
         <v>0.11751693494982141</v>
       </c>
       <c r="S4">
-        <f>M4 * SQRT(3 * (1 - P4))</f>
+        <f t="shared" si="0"/>
         <v>0.17965642209506727</v>
       </c>
       <c r="T4">
-        <f>N4 * SQRT(3 * (1 - Q4))</f>
+        <f t="shared" si="0"/>
         <v>0.25308344473710243</v>
       </c>
       <c r="U4">
-        <f xml:space="preserve"> 1 / R4</f>
+        <f t="shared" si="1"/>
         <v>8.5094118598905801</v>
       </c>
       <c r="V4">
-        <f xml:space="preserve"> 1 / S4</f>
+        <f t="shared" si="1"/>
         <v>5.5661800916353465</v>
       </c>
       <c r="W4">
-        <f xml:space="preserve"> 1 / T4</f>
+        <f t="shared" si="1"/>
         <v>3.9512659590941568</v>
       </c>
     </row>
@@ -743,15 +747,15 @@
         <v>1.6600000000000001</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.9350000000000001</v>
       </c>
       <c r="O5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.98821396192203093</v>
       </c>
       <c r="P5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.95783132530120474</v>
       </c>
       <c r="Q5">
@@ -759,38 +763,121 @@
         <v>0.92506459948320408</v>
       </c>
       <c r="R5">
-        <f>L5 * SQRT(3 * (1 - O5))</f>
+        <f t="shared" si="0"/>
         <v>0.20740540012256101</v>
       </c>
       <c r="S5">
-        <f>M5 * SQRT(3 * (1 - P5))</f>
+        <f t="shared" si="0"/>
         <v>0.59042357676502111</v>
       </c>
       <c r="T5">
-        <f>N5 * SQRT(3 * (1 - Q5))</f>
+        <f t="shared" si="0"/>
         <v>0.91745572100238204</v>
       </c>
       <c r="U5">
-        <f xml:space="preserve"> 1 / R5</f>
+        <f t="shared" si="1"/>
         <v>4.8214752335719089</v>
       </c>
       <c r="V5">
-        <f xml:space="preserve"> 1 / S5</f>
+        <f t="shared" si="1"/>
         <v>1.6936993022519213</v>
       </c>
       <c r="W5">
-        <f xml:space="preserve"> 1 / T5</f>
+        <f t="shared" si="1"/>
         <v>1.0899708586561898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>0.24</v>
+      </c>
+      <c r="C6">
+        <v>0.24</v>
+      </c>
+      <c r="D6">
+        <v>0.24</v>
+      </c>
+      <c r="E6">
+        <v>0.01</v>
+      </c>
+      <c r="F6">
+        <v>0.01</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0.9</v>
+      </c>
+      <c r="K6">
+        <v>1.5</v>
+      </c>
+      <c r="L6">
+        <f xml:space="preserve"> B6 + E6</f>
+        <v>0.25</v>
+      </c>
+      <c r="M6">
+        <f xml:space="preserve"> C6 + F6</f>
+        <v>0.25</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="3"/>
+        <v>0.96</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>0.96</v>
+      </c>
+      <c r="Q6">
+        <f>D6/N6</f>
+        <v>0.96</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>8.6602540378443907E-2</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>8.6602540378443907E-2</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>8.6602540378443907E-2</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="1"/>
+        <v>11.547005383792509</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="1"/>
+        <v>11.547005383792509</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="1"/>
+        <v>11.547005383792509</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="R1:T1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="R1:T1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>